<commit_message>
SSDM-13479: Mass-Merge of all XLS Import/Export updates
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-plain-text.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-plain-text.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t xml:space="preserve">DATASET</t>
   </si>
@@ -31,33 +31,96 @@
     <t xml:space="preserve">ATTACHMENT</t>
   </si>
   <si>
+    <t xml:space="preserve">PermId</t>
+  </si>
+  <si>
     <t xml:space="preserve">Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Archiving status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present in archive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage confirmation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample</t>
   </si>
   <si>
+    <t xml:space="preserve">Parents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Attachment</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0002</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEST_2</t>
   </si>
   <si>
+    <t xml:space="preserve">AVAILABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">/TEST/TEST_2</t>
   </si>
   <si>
+    <t xml:space="preserve">TEST_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-10 17:23:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;i&gt;Test 2&lt;/i&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">file1.bin</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEST_3</t>
   </si>
   <si>
+    <t xml:space="preserve">ARCHIVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">/TEST/TEST_3</t>
   </si>
   <si>
@@ -76,10 +139,14 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">TEST_1</t>
+    <t xml:space="preserve">200001010000000-0001</t>
   </si>
   <si>
     <t xml:space="preserve">/TEST/TEST_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST_2
+TEST_3</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;Test 1&lt;/b&gt;</t>
@@ -94,8 +161,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -186,36 +255,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,132 +317,303 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ12"/>
+  <dimension ref="A1:AMU12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="20.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1033" min="1033" style="1" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" s="9" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="J11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="K11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="M11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" s="6" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AMJ11" s="0"/>
+      <c r="N11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AMT11" s="1"/>
+      <c r="AMU11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D12" s="7" t="s">
-        <v>21</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>